<commit_message>
Inplement buy in patern.
</commit_message>
<xml_diff>
--- a/output/ship_rule_sell.xlsx
+++ b/output/ship_rule_sell.xlsx
@@ -383,33 +383,33 @@
         </is>
       </c>
       <c r="B1" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C1" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D1" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E1" s="0" t="n">
-        <v>300</v>
+        <v>900</v>
       </c>
       <c r="F1" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G1" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H1" s="0" t="inlineStr">
         <is>
-          <t>sell 25 ships</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I1" s="0" t="n">
-        <v>0.07756146449907203</v>
+        <v>0.3204544237914111</v>
       </c>
       <c r="J1" s="0" t="n">
-        <v>0</v>
+        <v>0.01941998882989721</v>
       </c>
     </row>
     <row r="2">
@@ -419,33 +419,33 @@
         </is>
       </c>
       <c r="B2" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>300</v>
+        <v>900</v>
       </c>
       <c r="F2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
-          <t>sell 25 ships</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I2" s="0" t="n">
-        <v>0.07756146449907203</v>
+        <v>0.3204544237914111</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>0</v>
+        <v>0.01941998882989721</v>
       </c>
     </row>
     <row r="3">
@@ -455,33 +455,33 @@
         </is>
       </c>
       <c r="B3" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H3" s="0" t="inlineStr">
         <is>
-          <t>sell 25 ships</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I3" s="0" t="n">
-        <v>0.07756146449907203</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="4">
@@ -491,33 +491,33 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>900</v>
       </c>
       <c r="F4" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H4" s="0" t="inlineStr">
         <is>
-          <t>sell 25 ships</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I4" s="0" t="n">
-        <v>0.07756146449907203</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="5">
@@ -527,33 +527,33 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="F5" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="F5" s="0" t="n">
+      <c r="G5" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H5" s="0" t="inlineStr">
         <is>
-          <t>sell 25 ships</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I5" s="0" t="n">
-        <v>0.07756146449907203</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="6">
@@ -563,33 +563,33 @@
         </is>
       </c>
       <c r="B6" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>300</v>
+        <v>900</v>
       </c>
       <c r="F6" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H6" s="0" t="inlineStr">
         <is>
-          <t>sell 25 ships</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I6" s="0" t="n">
-        <v>0.07756146449907203</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="7">
@@ -599,33 +599,33 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="F7" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="F7" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H7" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I7" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="8">
@@ -635,33 +635,33 @@
         </is>
       </c>
       <c r="B8" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="F8" s="0" t="n">
+      <c r="G8" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H8" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I8" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="9">
@@ -674,30 +674,30 @@
         <v>60</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H9" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I9" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="10">
@@ -710,30 +710,30 @@
         <v>60</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H10" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I10" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="11">
@@ -743,33 +743,33 @@
         </is>
       </c>
       <c r="B11" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H11" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I11" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="12">
@@ -782,30 +782,30 @@
         <v>60</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H12" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I12" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="13">
@@ -815,33 +815,33 @@
         </is>
       </c>
       <c r="B13" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="F13" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H13" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I13" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="14">
@@ -854,30 +854,30 @@
         <v>60</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H14" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I14" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="15">
@@ -887,33 +887,33 @@
         </is>
       </c>
       <c r="B15" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H15" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I15" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.3181411348090248</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>0</v>
+        <v>0.01949011034023529</v>
       </c>
     </row>
     <row r="16">
@@ -923,33 +923,33 @@
         </is>
       </c>
       <c r="B16" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H16" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I16" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.3038953799060413</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>0</v>
+        <v>0.01900299955649834</v>
       </c>
     </row>
     <row r="17">
@@ -959,33 +959,33 @@
         </is>
       </c>
       <c r="B17" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="H17" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 2 ships</t>
         </is>
       </c>
       <c r="I17" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2913480511707084</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>0</v>
+        <v>0.02616600606059722</v>
       </c>
     </row>
     <row r="18">
@@ -995,33 +995,33 @@
         </is>
       </c>
       <c r="B18" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H18" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I18" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2885228208789394</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>0</v>
+        <v>0.017360891699831</v>
       </c>
     </row>
     <row r="19">
@@ -1031,33 +1031,33 @@
         </is>
       </c>
       <c r="B19" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H19" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I19" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2885228208789394</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>0</v>
+        <v>0.017360891699831</v>
       </c>
     </row>
     <row r="20">
@@ -1067,33 +1067,33 @@
         </is>
       </c>
       <c r="B20" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H20" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I20" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2874918590222748</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>0</v>
+        <v>0.01709027399497428</v>
       </c>
     </row>
     <row r="21">
@@ -1106,30 +1106,30 @@
         <v>60</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H21" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I21" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2874918590222748</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>0</v>
+        <v>0.01709027399497428</v>
       </c>
     </row>
     <row r="22">
@@ -1142,30 +1142,30 @@
         <v>60</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H22" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I22" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2874918590222748</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>0</v>
+        <v>0.01709027399497428</v>
       </c>
     </row>
     <row r="23">
@@ -1175,33 +1175,33 @@
         </is>
       </c>
       <c r="B23" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="F23" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C23" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="G23" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H23" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I23" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2874918590222748</v>
       </c>
       <c r="J23" s="0" t="n">
-        <v>0</v>
+        <v>0.01709027399497428</v>
       </c>
     </row>
     <row r="24">
@@ -1211,33 +1211,33 @@
         </is>
       </c>
       <c r="B24" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H24" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I24" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2874918590222748</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>0</v>
+        <v>0.01709027399497428</v>
       </c>
     </row>
     <row r="25">
@@ -1247,33 +1247,33 @@
         </is>
       </c>
       <c r="B25" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="F25" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C25" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>130</v>
-      </c>
       <c r="G25" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H25" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I25" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2874918590222748</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>0</v>
+        <v>0.01709027399497428</v>
       </c>
     </row>
     <row r="26">
@@ -1283,33 +1283,33 @@
         </is>
       </c>
       <c r="B26" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H26" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I26" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2867705454529071</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>0</v>
+        <v>0.01763773929827899</v>
       </c>
     </row>
     <row r="27">
@@ -1319,33 +1319,33 @@
         </is>
       </c>
       <c r="B27" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H27" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I27" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2867705454529071</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>0</v>
+        <v>0.01763773929827899</v>
       </c>
     </row>
     <row r="28">
@@ -1355,33 +1355,33 @@
         </is>
       </c>
       <c r="B28" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H28" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I28" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2867705454529071</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>0</v>
+        <v>0.01763773929827899</v>
       </c>
     </row>
     <row r="29">
@@ -1394,30 +1394,30 @@
         <v>60</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H29" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I29" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2867705454529071</v>
       </c>
       <c r="J29" s="0" t="n">
-        <v>0</v>
+        <v>0.01763773929827899</v>
       </c>
     </row>
     <row r="30">
@@ -1427,33 +1427,33 @@
         </is>
       </c>
       <c r="B30" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H30" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I30" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2867705454529071</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>0</v>
+        <v>0.01763773929827899</v>
       </c>
     </row>
     <row r="31">
@@ -1463,33 +1463,33 @@
         </is>
       </c>
       <c r="B31" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H31" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I31" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2867705454529071</v>
       </c>
       <c r="J31" s="0" t="n">
-        <v>0</v>
+        <v>0.01763773929827899</v>
       </c>
     </row>
     <row r="32">
@@ -1502,30 +1502,30 @@
         <v>60</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H32" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I32" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2867705454529071</v>
       </c>
       <c r="J32" s="0" t="n">
-        <v>0</v>
+        <v>0.01763773929827899</v>
       </c>
     </row>
     <row r="33">
@@ -1535,33 +1535,33 @@
         </is>
       </c>
       <c r="B33" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H33" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I33" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2867705454529071</v>
       </c>
       <c r="J33" s="0" t="n">
-        <v>0</v>
+        <v>0.01763773929827899</v>
       </c>
     </row>
     <row r="34">
@@ -1571,33 +1571,33 @@
         </is>
       </c>
       <c r="B34" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H34" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I34" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2470113386759419</v>
       </c>
       <c r="J34" s="0" t="n">
-        <v>0</v>
+        <v>0.009998429612980237</v>
       </c>
     </row>
     <row r="35">
@@ -1607,33 +1607,33 @@
         </is>
       </c>
       <c r="B35" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F35" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C35" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="F35" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="G35" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H35" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I35" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2466551132558966</v>
       </c>
       <c r="J35" s="0" t="n">
-        <v>0</v>
+        <v>0.009727657670405503</v>
       </c>
     </row>
     <row r="36">
@@ -1643,33 +1643,33 @@
         </is>
       </c>
       <c r="B36" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F36" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C36" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="D36" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E36" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="G36" s="0" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H36" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I36" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2466551132558966</v>
       </c>
       <c r="J36" s="0" t="n">
-        <v>0</v>
+        <v>0.009727657670405503</v>
       </c>
     </row>
     <row r="37">
@@ -1679,33 +1679,33 @@
         </is>
       </c>
       <c r="B37" s="0" t="n">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>300</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>800</v>
+        <v>1500</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H37" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I37" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2461515963975854</v>
       </c>
       <c r="J37" s="0" t="n">
-        <v>0</v>
+        <v>0.009827233815905376</v>
       </c>
     </row>
     <row r="38">
@@ -1715,33 +1715,33 @@
         </is>
       </c>
       <c r="B38" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H38" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I38" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2461515963975854</v>
       </c>
       <c r="J38" s="0" t="n">
-        <v>0</v>
+        <v>0.009827233815905376</v>
       </c>
     </row>
     <row r="39">
@@ -1751,33 +1751,33 @@
         </is>
       </c>
       <c r="B39" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H39" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I39" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2461515963975854</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>0</v>
+        <v>0.009827233815905376</v>
       </c>
     </row>
     <row r="40">
@@ -1787,33 +1787,33 @@
         </is>
       </c>
       <c r="B40" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H40" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I40" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2461515963975854</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>0</v>
+        <v>0.009827233815905376</v>
       </c>
     </row>
     <row r="41">
@@ -1823,33 +1823,33 @@
         </is>
       </c>
       <c r="B41" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H41" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I41" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2461515963975854</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>0</v>
+        <v>0.009827233815905376</v>
       </c>
     </row>
     <row r="42">
@@ -1859,33 +1859,33 @@
         </is>
       </c>
       <c r="B42" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>300</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="G42" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H42" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I42" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.2461515963975854</v>
       </c>
       <c r="J42" s="0" t="n">
-        <v>0</v>
+        <v>0.009827233815905376</v>
       </c>
     </row>
     <row r="43">
@@ -1895,33 +1895,33 @@
         </is>
       </c>
       <c r="B43" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H43" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 2 ships</t>
         </is>
       </c>
       <c r="I43" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.1850013701023207</v>
       </c>
       <c r="J43" s="0" t="n">
-        <v>0</v>
+        <v>0.006890306021656628</v>
       </c>
     </row>
     <row r="44">
@@ -1931,33 +1931,33 @@
         </is>
       </c>
       <c r="B44" s="0" t="n">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E44" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="G44" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H44" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 2 ships</t>
         </is>
       </c>
       <c r="I44" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.1850013701023207</v>
       </c>
       <c r="J44" s="0" t="n">
-        <v>0</v>
+        <v>0.006890306021656628</v>
       </c>
     </row>
     <row r="45">
@@ -1967,33 +1967,33 @@
         </is>
       </c>
       <c r="B45" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>1100</v>
+      </c>
+      <c r="F45" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C45" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>700</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="G45" s="0" t="n">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="H45" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 1 ships</t>
         </is>
       </c>
       <c r="I45" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.1707172992499822</v>
       </c>
       <c r="J45" s="0" t="n">
-        <v>0</v>
+        <v>0.02050015088135129</v>
       </c>
     </row>
     <row r="46">
@@ -2003,33 +2003,33 @@
         </is>
       </c>
       <c r="B46" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C46" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C46" s="0" t="n">
-        <v>130</v>
-      </c>
       <c r="D46" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H46" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 2 ships</t>
         </is>
       </c>
       <c r="I46" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.1195592491225005</v>
       </c>
       <c r="J46" s="0" t="n">
-        <v>0</v>
+        <v>0.001075821145733432</v>
       </c>
     </row>
     <row r="47">
@@ -2039,33 +2039,33 @@
         </is>
       </c>
       <c r="B47" s="0" t="n">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C47" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="G47" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="D47" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E47" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="F47" s="0" t="n">
-        <v>110</v>
-      </c>
-      <c r="G47" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H47" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 2 ships</t>
         </is>
       </c>
       <c r="I47" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.1195592491225005</v>
       </c>
       <c r="J47" s="0" t="n">
-        <v>0</v>
+        <v>0.001075821145733432</v>
       </c>
     </row>
     <row r="48">
@@ -2075,33 +2075,33 @@
         </is>
       </c>
       <c r="B48" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C48" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C48" s="0" t="n">
-        <v>130</v>
-      </c>
       <c r="D48" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="G48" s="0" t="n">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H48" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 2 ships</t>
         </is>
       </c>
       <c r="I48" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.1195592491225005</v>
       </c>
       <c r="J48" s="0" t="n">
-        <v>0</v>
+        <v>0.001075821145733432</v>
       </c>
     </row>
     <row r="49">
@@ -2111,33 +2111,33 @@
         </is>
       </c>
       <c r="B49" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>130</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>300</v>
+        <v>900</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="G49" s="0" t="n">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="H49" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 70 ships</t>
         </is>
       </c>
       <c r="I49" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.08243735745583118</v>
       </c>
       <c r="J49" s="0" t="n">
-        <v>0</v>
+        <v>0.0007600933360426019</v>
       </c>
     </row>
     <row r="50">
@@ -2147,33 +2147,33 @@
         </is>
       </c>
       <c r="B50" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>130</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>300</v>
+        <v>900</v>
       </c>
       <c r="E50" s="0" t="n">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>160</v>
       </c>
       <c r="H50" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 70 ships</t>
         </is>
       </c>
       <c r="I50" s="0" t="n">
-        <v>-0.2486559791615969</v>
+        <v>0.08243735745583118</v>
       </c>
       <c r="J50" s="0" t="n">
-        <v>0</v>
+        <v>0.0007600933360426019</v>
       </c>
     </row>
     <row r="51">
@@ -2183,31 +2183,33 @@
         </is>
       </c>
       <c r="B51" s="0" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>60</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G51" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="H51" s="0" t="n">
-        <v>60</v>
+        <v>110</v>
+      </c>
+      <c r="H51" s="0" t="inlineStr">
+        <is>
+          <t>sell 10 ships</t>
+        </is>
       </c>
       <c r="I51" s="0" t="n">
-        <v>-0.06272551091992508</v>
+        <v>-0.06397604419277692</v>
       </c>
       <c r="J51" s="0" t="n">
-        <v>0.0005029477746801888</v>
+        <v>4.843684143957145e-05</v>
       </c>
     </row>
     <row r="52">
@@ -2217,31 +2219,33 @@
         </is>
       </c>
       <c r="B52" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>900</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="G52" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="H52" s="0" t="n">
-        <v>70</v>
+        <v>200</v>
+      </c>
+      <c r="H52" s="0" t="inlineStr">
+        <is>
+          <t>sell 70 ships</t>
+        </is>
       </c>
       <c r="I52" s="0" t="n">
-        <v>-0.06290426594238022</v>
+        <v>-0.08442976718711787</v>
       </c>
       <c r="J52" s="0" t="n">
-        <v>0.0003962507817838435</v>
+        <v>7.644114424754522e-05</v>
       </c>
     </row>
     <row r="53">
@@ -2254,10 +2258,10 @@
         <v>0</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>300</v>
+        <v>700</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>1300</v>
@@ -2266,16 +2270,18 @@
         <v>70</v>
       </c>
       <c r="G53" s="0" t="n">
-        <v>160</v>
-      </c>
-      <c r="H53" s="0" t="n">
-        <v>40</v>
+        <v>120</v>
+      </c>
+      <c r="H53" s="0" t="inlineStr">
+        <is>
+          <t>sell 30 ships</t>
+        </is>
       </c>
       <c r="I53" s="0" t="n">
-        <v>-0.0682770214178765</v>
+        <v>-0.08976615527610522</v>
       </c>
       <c r="J53" s="0" t="n">
-        <v>0.000535194739130279</v>
+        <v>0.0002981373797873592</v>
       </c>
     </row>
     <row r="54">
@@ -2285,31 +2291,33 @@
         </is>
       </c>
       <c r="B54" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>300</v>
+        <v>700</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>1200</v>
+        <v>1800</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="G54" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="H54" s="0" t="n">
-        <v>40</v>
+        <v>120</v>
+      </c>
+      <c r="H54" s="0" t="inlineStr">
+        <is>
+          <t>sell 30 ships</t>
+        </is>
       </c>
       <c r="I54" s="0" t="n">
-        <v>-0.0682770214178765</v>
+        <v>-0.08976615527610522</v>
       </c>
       <c r="J54" s="0" t="n">
-        <v>0.000535194739130279</v>
+        <v>0.0002981373797873592</v>
       </c>
     </row>
     <row r="55">
@@ -2319,31 +2327,33 @@
         </is>
       </c>
       <c r="B55" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>700</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>1200</v>
+        <v>1500</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="G55" s="0" t="n">
-        <v>110</v>
-      </c>
-      <c r="H55" s="0" t="n">
-        <v>50</v>
+        <v>120</v>
+      </c>
+      <c r="H55" s="0" t="inlineStr">
+        <is>
+          <t>sell 30 ships</t>
+        </is>
       </c>
       <c r="I55" s="0" t="n">
-        <v>-0.06877803870576686</v>
+        <v>-0.08976615527610522</v>
       </c>
       <c r="J55" s="0" t="n">
-        <v>0.0004663348511805455</v>
+        <v>0.0002981373797873592</v>
       </c>
     </row>
     <row r="56">
@@ -2353,31 +2363,33 @@
         </is>
       </c>
       <c r="B56" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>700</v>
       </c>
       <c r="E56" s="0" t="n">
-        <v>1100</v>
+        <v>1300</v>
       </c>
       <c r="F56" s="0" t="n">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="G56" s="0" t="n">
-        <v>160</v>
-      </c>
-      <c r="H56" s="0" t="n">
-        <v>50</v>
+        <v>120</v>
+      </c>
+      <c r="H56" s="0" t="inlineStr">
+        <is>
+          <t>sell 30 ships</t>
+        </is>
       </c>
       <c r="I56" s="0" t="n">
-        <v>-0.06877803870576686</v>
+        <v>-0.08976615527610522</v>
       </c>
       <c r="J56" s="0" t="n">
-        <v>0.0004663348511805455</v>
+        <v>0.0002981373797873592</v>
       </c>
     </row>
     <row r="57">
@@ -2387,31 +2399,33 @@
         </is>
       </c>
       <c r="B57" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>700</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>60</v>
       </c>
       <c r="G57" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="H57" s="0" t="n">
-        <v>20</v>
+        <v>120</v>
+      </c>
+      <c r="H57" s="0" t="inlineStr">
+        <is>
+          <t>sell 30 ships</t>
+        </is>
       </c>
       <c r="I57" s="0" t="n">
-        <v>-0.06898115321392184</v>
+        <v>-0.08976615527610522</v>
       </c>
       <c r="J57" s="0" t="n">
-        <v>0.0006408076172447999</v>
+        <v>0.0002981373797873592</v>
       </c>
     </row>
     <row r="58">
@@ -2421,31 +2435,33 @@
         </is>
       </c>
       <c r="B58" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>700</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="F58" s="0" t="n">
         <v>60</v>
       </c>
       <c r="G58" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="H58" s="0" t="n">
-        <v>20</v>
+        <v>120</v>
+      </c>
+      <c r="H58" s="0" t="inlineStr">
+        <is>
+          <t>sell 30 ships</t>
+        </is>
       </c>
       <c r="I58" s="0" t="n">
-        <v>-0.06898115321392184</v>
+        <v>-0.08976615527610522</v>
       </c>
       <c r="J58" s="0" t="n">
-        <v>0.0006408076172447999</v>
+        <v>0.0002981373797873592</v>
       </c>
     </row>
     <row r="59">
@@ -2458,28 +2474,30 @@
         <v>0</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>1400</v>
+        <v>700</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="G59" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="H59" s="0" t="n">
-        <v>25</v>
+        <v>120</v>
+      </c>
+      <c r="H59" s="0" t="inlineStr">
+        <is>
+          <t>sell 30 ships</t>
+        </is>
       </c>
       <c r="I59" s="0" t="n">
-        <v>-0.06906556169774257</v>
+        <v>-0.08976615527610522</v>
       </c>
       <c r="J59" s="0" t="n">
-        <v>0.0005554342234644088</v>
+        <v>0.0002981373797873592</v>
       </c>
     </row>
     <row r="60">
@@ -2489,31 +2507,33 @@
         </is>
       </c>
       <c r="B60" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>900</v>
+        <v>1300</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="G60" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="H60" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
+      </c>
+      <c r="H60" s="0" t="inlineStr">
+        <is>
+          <t>sell 30 ships</t>
+        </is>
       </c>
       <c r="I60" s="0" t="n">
-        <v>-0.0695704208008063</v>
+        <v>-0.08976615527610522</v>
       </c>
       <c r="J60" s="0" t="n">
-        <v>0.000245508443654629</v>
+        <v>0.0002981373797873592</v>
       </c>
     </row>
     <row r="61">
@@ -2523,31 +2543,33 @@
         </is>
       </c>
       <c r="B61" s="0" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G61" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="H61" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
+      </c>
+      <c r="H61" s="0" t="inlineStr">
+        <is>
+          <t>sell 30 ships</t>
+        </is>
       </c>
       <c r="I61" s="0" t="n">
-        <v>-0.0695704208008063</v>
+        <v>-0.08976615527610522</v>
       </c>
       <c r="J61" s="0" t="n">
-        <v>0.000245508443654629</v>
+        <v>0.0002981373797873592</v>
       </c>
     </row>
     <row r="62">
@@ -2557,31 +2579,33 @@
         </is>
       </c>
       <c r="B62" s="0" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="E62" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G62" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="H62" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
+      </c>
+      <c r="H62" s="0" t="inlineStr">
+        <is>
+          <t>sell 30 ships</t>
+        </is>
       </c>
       <c r="I62" s="0" t="n">
-        <v>-0.0695704208008063</v>
+        <v>-0.08976615527610522</v>
       </c>
       <c r="J62" s="0" t="n">
-        <v>0.000245508443654629</v>
+        <v>0.0002981373797873592</v>
       </c>
     </row>
     <row r="63">
@@ -2591,31 +2615,33 @@
         </is>
       </c>
       <c r="B63" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>300</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G63" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="H63" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
+      </c>
+      <c r="H63" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
       <c r="I63" s="0" t="n">
-        <v>-0.06976851632456607</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J63" s="0" t="n">
-        <v>0.0002343702015025968</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="64">
@@ -2625,31 +2651,33 @@
         </is>
       </c>
       <c r="B64" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E64" s="0" t="n">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G64" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="H64" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
+      </c>
+      <c r="H64" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
       <c r="I64" s="0" t="n">
-        <v>-0.06976851632456607</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J64" s="0" t="n">
-        <v>0.0002343702015025968</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="65">
@@ -2659,31 +2687,33 @@
         </is>
       </c>
       <c r="B65" s="0" t="n">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>300</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="F65" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G65" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="H65" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
+      </c>
+      <c r="H65" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
       <c r="I65" s="0" t="n">
-        <v>-0.06976851632456607</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J65" s="0" t="n">
-        <v>0.0002343702015025968</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="66">
@@ -2693,31 +2723,33 @@
         </is>
       </c>
       <c r="B66" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>2000</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="G66" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="H66" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
+      </c>
+      <c r="H66" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
       <c r="I66" s="0" t="n">
-        <v>-0.06976851632456607</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J66" s="0" t="n">
-        <v>0.0002343702015025968</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="67">
@@ -2727,31 +2759,33 @@
         </is>
       </c>
       <c r="B67" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>1100</v>
+        <v>2000</v>
       </c>
       <c r="F67" s="0" t="n">
         <v>90</v>
       </c>
       <c r="G67" s="0" t="n">
-        <v>160</v>
-      </c>
-      <c r="H67" s="0" t="n">
-        <v>25</v>
+        <v>150</v>
+      </c>
+      <c r="H67" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
       <c r="I67" s="0" t="n">
-        <v>-0.07031219868448799</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J67" s="0" t="n">
-        <v>0.0004811326601273957</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="68">
@@ -2761,31 +2795,33 @@
         </is>
       </c>
       <c r="B68" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E68" s="0" t="n">
-        <v>1100</v>
+        <v>2000</v>
       </c>
       <c r="F68" s="0" t="n">
         <v>90</v>
       </c>
       <c r="G68" s="0" t="n">
-        <v>160</v>
-      </c>
-      <c r="H68" s="0" t="n">
-        <v>25</v>
+        <v>150</v>
+      </c>
+      <c r="H68" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
       <c r="I68" s="0" t="n">
-        <v>-0.07031219868448799</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J68" s="0" t="n">
-        <v>0.0004811326601273957</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="69">
@@ -2795,22 +2831,22 @@
         </is>
       </c>
       <c r="B69" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>2000</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G69" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="H69" s="0" t="inlineStr">
         <is>
@@ -2818,10 +2854,10 @@
         </is>
       </c>
       <c r="I69" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J69" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="70">
@@ -2831,22 +2867,22 @@
         </is>
       </c>
       <c r="B70" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="E70" s="0" t="n">
-        <v>300</v>
+        <v>3000</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="G70" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H70" s="0" t="inlineStr">
         <is>
@@ -2854,10 +2890,10 @@
         </is>
       </c>
       <c r="I70" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J70" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="71">
@@ -2867,22 +2903,22 @@
         </is>
       </c>
       <c r="B71" s="0" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>500</v>
+        <v>1300</v>
       </c>
       <c r="E71" s="0" t="n">
-        <v>1400</v>
+        <v>3000</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="G71" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H71" s="0" t="inlineStr">
         <is>
@@ -2890,10 +2926,10 @@
         </is>
       </c>
       <c r="I71" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J71" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="72">
@@ -2903,22 +2939,22 @@
         </is>
       </c>
       <c r="B72" s="0" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>1500</v>
+        <v>300</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>2000</v>
       </c>
       <c r="F72" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G72" s="0" t="n">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="H72" s="0" t="inlineStr">
         <is>
@@ -2926,10 +2962,10 @@
         </is>
       </c>
       <c r="I72" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J72" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="73">
@@ -2939,22 +2975,22 @@
         </is>
       </c>
       <c r="B73" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F73" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="C73" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="D73" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="E73" s="0" t="n">
-        <v>1400</v>
-      </c>
-      <c r="F73" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="G73" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H73" s="0" t="inlineStr">
         <is>
@@ -2962,10 +2998,10 @@
         </is>
       </c>
       <c r="I73" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J73" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="74">
@@ -2975,33 +3011,33 @@
         </is>
       </c>
       <c r="B74" s="0" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="C74" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="G74" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D74" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E74" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="F74" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="G74" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H74" s="0" t="inlineStr">
         <is>
           <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I74" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J74" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="75">
@@ -3011,22 +3047,22 @@
         </is>
       </c>
       <c r="B75" s="0" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="E75" s="0" t="n">
-        <v>1400</v>
+        <v>3000</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="G75" s="0" t="n">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="H75" s="0" t="inlineStr">
         <is>
@@ -3034,10 +3070,10 @@
         </is>
       </c>
       <c r="I75" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J75" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="76">
@@ -3047,22 +3083,22 @@
         </is>
       </c>
       <c r="B76" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="E76" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F76" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="G76" s="0" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="H76" s="0" t="inlineStr">
         <is>
@@ -3070,10 +3106,10 @@
         </is>
       </c>
       <c r="I76" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J76" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="77">
@@ -3083,33 +3119,33 @@
         </is>
       </c>
       <c r="B77" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G77" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C77" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="D77" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="E77" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="F77" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G77" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="H77" s="0" t="inlineStr">
         <is>
           <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I77" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J77" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="78">
@@ -3119,33 +3155,33 @@
         </is>
       </c>
       <c r="B78" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F78" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C78" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="D78" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="E78" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F78" s="0" t="n">
+      <c r="G78" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="G78" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H78" s="0" t="inlineStr">
         <is>
           <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I78" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J78" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="79">
@@ -3155,22 +3191,22 @@
         </is>
       </c>
       <c r="B79" s="0" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E79" s="0" t="n">
-        <v>300</v>
+        <v>900</v>
       </c>
       <c r="F79" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G79" s="0" t="n">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="H79" s="0" t="inlineStr">
         <is>
@@ -3178,10 +3214,10 @@
         </is>
       </c>
       <c r="I79" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J79" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="80">
@@ -3191,22 +3227,22 @@
         </is>
       </c>
       <c r="B80" s="0" t="n">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="E80" s="0" t="n">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="F80" s="0" t="n">
         <v>80</v>
       </c>
       <c r="G80" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H80" s="0" t="inlineStr">
         <is>
@@ -3214,10 +3250,10 @@
         </is>
       </c>
       <c r="I80" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J80" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="81">
@@ -3227,22 +3263,22 @@
         </is>
       </c>
       <c r="B81" s="0" t="n">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E81" s="0" t="n">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="F81" s="0" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="G81" s="0" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H81" s="0" t="inlineStr">
         <is>
@@ -3250,10 +3286,10 @@
         </is>
       </c>
       <c r="I81" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J81" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="82">
@@ -3263,22 +3299,22 @@
         </is>
       </c>
       <c r="B82" s="0" t="n">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C82" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F82" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="D82" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="E82" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="F82" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="G82" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="H82" s="0" t="inlineStr">
         <is>
@@ -3286,10 +3322,10 @@
         </is>
       </c>
       <c r="I82" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J82" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="83">
@@ -3299,31 +3335,33 @@
         </is>
       </c>
       <c r="B83" s="0" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>90</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>1300</v>
+        <v>300</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>2000</v>
       </c>
       <c r="F83" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="G83" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="H83" s="0" t="n">
-        <v>0</v>
+        <v>150</v>
+      </c>
+      <c r="H83" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
       <c r="I83" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J83" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="84">
@@ -3333,13 +3371,13 @@
         </is>
       </c>
       <c r="B84" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>800</v>
+        <v>1500</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>1500</v>
@@ -3348,7 +3386,7 @@
         <v>80</v>
       </c>
       <c r="G84" s="0" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="H84" s="0" t="inlineStr">
         <is>
@@ -3356,10 +3394,10 @@
         </is>
       </c>
       <c r="I84" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J84" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="85">
@@ -3369,33 +3407,33 @@
         </is>
       </c>
       <c r="B85" s="0" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C85" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G85" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D85" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="E85" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="F85" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="G85" s="0" t="n">
-        <v>140</v>
-      </c>
       <c r="H85" s="0" t="inlineStr">
         <is>
           <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I85" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J85" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="86">
@@ -3405,19 +3443,19 @@
         </is>
       </c>
       <c r="B86" s="0" t="n">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E86" s="0" t="n">
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="F86" s="0" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="G86" s="0" t="n">
         <v>150</v>
@@ -3428,10 +3466,10 @@
         </is>
       </c>
       <c r="I86" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J86" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="87">
@@ -3441,22 +3479,22 @@
         </is>
       </c>
       <c r="B87" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C87" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C87" s="0" t="n">
-        <v>140</v>
-      </c>
       <c r="D87" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E87" s="0" t="n">
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="F87" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G87" s="0" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="H87" s="0" t="inlineStr">
         <is>
@@ -3464,10 +3502,10 @@
         </is>
       </c>
       <c r="I87" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J87" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="88">
@@ -3477,22 +3515,22 @@
         </is>
       </c>
       <c r="B88" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="E88" s="0" t="n">
-        <v>1400</v>
+        <v>3000</v>
       </c>
       <c r="F88" s="0" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G88" s="0" t="n">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="H88" s="0" t="inlineStr">
         <is>
@@ -3500,10 +3538,10 @@
         </is>
       </c>
       <c r="I88" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J88" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="89">
@@ -3516,19 +3554,19 @@
         <v>60</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="E89" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
       <c r="F89" s="0" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="G89" s="0" t="n">
-        <v>200</v>
+        <v>130</v>
       </c>
       <c r="H89" s="0" t="inlineStr">
         <is>
@@ -3536,10 +3574,10 @@
         </is>
       </c>
       <c r="I89" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J89" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="90">
@@ -3549,22 +3587,22 @@
         </is>
       </c>
       <c r="B90" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E90" s="0" t="n">
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="F90" s="0" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="G90" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H90" s="0" t="inlineStr">
         <is>
@@ -3572,10 +3610,10 @@
         </is>
       </c>
       <c r="I90" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J90" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="91">
@@ -3585,22 +3623,22 @@
         </is>
       </c>
       <c r="B91" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>300</v>
+        <v>800</v>
       </c>
       <c r="E91" s="0" t="n">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="F91" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G91" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="H91" s="0" t="inlineStr">
         <is>
@@ -3608,10 +3646,10 @@
         </is>
       </c>
       <c r="I91" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J91" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="92">
@@ -3621,22 +3659,22 @@
         </is>
       </c>
       <c r="B92" s="0" t="n">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="C92" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F92" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="D92" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E92" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F92" s="0" t="n">
-        <v>90</v>
-      </c>
       <c r="G92" s="0" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H92" s="0" t="inlineStr">
         <is>
@@ -3644,10 +3682,10 @@
         </is>
       </c>
       <c r="I92" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J92" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="93">
@@ -3657,22 +3695,22 @@
         </is>
       </c>
       <c r="B93" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E93" s="0" t="n">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G93" s="0" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="H93" s="0" t="inlineStr">
         <is>
@@ -3680,10 +3718,10 @@
         </is>
       </c>
       <c r="I93" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J93" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="94">
@@ -3693,22 +3731,22 @@
         </is>
       </c>
       <c r="B94" s="0" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="E94" s="0" t="n">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>70</v>
+        <v>160</v>
       </c>
       <c r="G94" s="0" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="H94" s="0" t="inlineStr">
         <is>
@@ -3716,10 +3754,10 @@
         </is>
       </c>
       <c r="I94" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J94" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="95">
@@ -3729,22 +3767,22 @@
         </is>
       </c>
       <c r="B95" s="0" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E95" s="0" t="n">
-        <v>1500</v>
+        <v>1300</v>
       </c>
       <c r="F95" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="G95" s="0" t="n">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="H95" s="0" t="inlineStr">
         <is>
@@ -3752,10 +3790,10 @@
         </is>
       </c>
       <c r="I95" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J95" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="96">
@@ -3768,19 +3806,19 @@
         <v>10</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>1100</v>
+        <v>600</v>
       </c>
       <c r="E96" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="F96" s="0" t="n">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="G96" s="0" t="n">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="H96" s="0" t="inlineStr">
         <is>
@@ -3788,10 +3826,10 @@
         </is>
       </c>
       <c r="I96" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J96" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="97">
@@ -3801,19 +3839,19 @@
         </is>
       </c>
       <c r="B97" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>900</v>
+        <v>300</v>
       </c>
       <c r="E97" s="0" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="F97" s="0" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="G97" s="0" t="n">
         <v>130</v>
@@ -3824,10 +3862,10 @@
         </is>
       </c>
       <c r="I97" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J97" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="98">
@@ -3837,31 +3875,33 @@
         </is>
       </c>
       <c r="B98" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D98" s="0" t="n">
         <v>600</v>
       </c>
       <c r="E98" s="0" t="n">
-        <v>1800</v>
+        <v>900</v>
       </c>
       <c r="F98" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G98" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="H98" s="0" t="n">
-        <v>0</v>
+        <v>110</v>
+      </c>
+      <c r="H98" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
       <c r="I98" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J98" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="99">
@@ -3871,22 +3911,22 @@
         </is>
       </c>
       <c r="B99" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C99" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F99" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="D99" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E99" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F99" s="0" t="n">
-        <v>60</v>
-      </c>
       <c r="G99" s="0" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H99" s="0" t="inlineStr">
         <is>
@@ -3894,10 +3934,10 @@
         </is>
       </c>
       <c r="I99" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J99" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="100">
@@ -3907,22 +3947,22 @@
         </is>
       </c>
       <c r="B100" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>2000</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G100" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="H100" s="0" t="inlineStr">
         <is>
@@ -3930,10 +3970,10 @@
         </is>
       </c>
       <c r="I100" s="0" t="n">
-        <v>-0.07560613012344837</v>
+        <v>-0.1208794106022859</v>
       </c>
       <c r="J100" s="0" t="n">
-        <v>0.325116652034697</v>
+        <v>0.01632685147279231</v>
       </c>
     </row>
     <row r="101">

</xml_diff>